<commit_message>
Now does a pretty decent job of making an excel report on the result
</commit_message>
<xml_diff>
--- a/overrides.xlsx
+++ b/overrides.xlsx
@@ -20,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t xml:space="preserve">Rules are processed in order by the finance app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magic value program uses for some purpose internally</t>
   </si>
   <si>
     <t xml:space="preserve">R:</t>
@@ -215,13 +209,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ21"/>
+  <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -268,142 +262,133 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AMJ6" s="0"/>
-    </row>
-    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMJ7" s="0"/>
-    </row>
-    <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AMJ8" s="0"/>
-    </row>
-    <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="B11" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="AMJ10" s="0"/>
+      <c r="C11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2343</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>2343</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>22</v>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1171</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>23</v>
+      <c r="D19" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>